<commit_message>
Deploying to gh-pages from  @ 43b7990721c33768c7548478c2ac93332d74fee2 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_4-4-1.xlsx
+++ b/assets/excel/2021_4-4-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA11449A-E3A8-4BAE-B5CF-C38F635C9AE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0DC57C-1596-4F6F-9EA6-FC2564AF2FF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{0F19F7A8-EB0C-47DC-83FF-C18142F79EEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="49">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -508,72 +508,11 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -657,6 +596,67 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -976,8 +976,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B1:W74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,2178 +1006,2171 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
     </row>
     <row r="5" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
     </row>
     <row r="7" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14" t="s">
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="15" t="s">
+      <c r="N7" s="57" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
+      <c r="M8" s="44"/>
+      <c r="N8" s="57"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="57"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="B10" s="48"/>
+      <c r="C10" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
     </row>
     <row r="12" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L12" s="27" t="s">
+      <c r="L12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="M12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="27" t="s">
+      <c r="N12" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="9">
         <v>2020</v>
       </c>
-      <c r="E13" s="30">
+      <c r="E13" s="10">
         <v>2943</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="10">
         <v>2439</v>
       </c>
-      <c r="G13" s="30">
+      <c r="G13" s="10">
         <v>1182</v>
       </c>
-      <c r="H13" s="30">
+      <c r="H13" s="10">
         <v>900</v>
       </c>
-      <c r="I13" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J13" s="31">
+      <c r="I13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="11">
         <v>285</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="11">
         <v>3</v>
       </c>
-      <c r="L13" s="30">
+      <c r="L13" s="10">
         <v>69</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="11">
         <v>96</v>
       </c>
-      <c r="N13" s="30">
+      <c r="N13" s="10">
         <v>405</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="9">
         <v>2020</v>
       </c>
-      <c r="E14" s="30">
+      <c r="E14" s="10">
         <v>4008</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="10">
         <v>3087</v>
       </c>
-      <c r="G14" s="30">
+      <c r="G14" s="10">
         <v>1338</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="10">
         <v>1533</v>
       </c>
-      <c r="I14" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="31">
+      <c r="I14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="11">
         <v>84</v>
       </c>
-      <c r="K14" s="31">
+      <c r="K14" s="11">
         <v>27</v>
       </c>
-      <c r="L14" s="30">
+      <c r="L14" s="10">
         <v>108</v>
       </c>
-      <c r="M14" s="31">
+      <c r="M14" s="11">
         <v>132</v>
       </c>
-      <c r="N14" s="30">
+      <c r="N14" s="10">
         <v>786</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="13">
         <v>2020</v>
       </c>
-      <c r="E15" s="34">
+      <c r="E15" s="14">
         <v>6951</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="14">
         <v>5529</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="14">
         <v>2520</v>
       </c>
-      <c r="H15" s="34">
+      <c r="H15" s="14">
         <v>2433</v>
       </c>
-      <c r="I15" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J15" s="30">
+      <c r="I15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="10">
         <v>369</v>
       </c>
-      <c r="K15" s="30">
+      <c r="K15" s="10">
         <v>30</v>
       </c>
-      <c r="L15" s="34">
+      <c r="L15" s="14">
         <v>174</v>
       </c>
-      <c r="M15" s="30">
+      <c r="M15" s="10">
         <v>231</v>
       </c>
-      <c r="N15" s="34">
+      <c r="N15" s="14">
         <v>1191</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D16" s="9">
         <v>2020</v>
       </c>
-      <c r="E16" s="30">
+      <c r="E16" s="10">
         <v>1902</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="10">
         <v>1614</v>
       </c>
-      <c r="G16" s="30">
+      <c r="G16" s="10">
         <v>747</v>
       </c>
-      <c r="H16" s="30">
+      <c r="H16" s="10">
         <v>855</v>
       </c>
-      <c r="I16" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L16" s="30">
+      <c r="I16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="10">
         <v>12</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M16" s="11">
         <v>36</v>
       </c>
-      <c r="N16" s="30">
+      <c r="N16" s="10">
         <v>252</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="9">
         <v>2020</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="10">
         <v>3225</v>
       </c>
-      <c r="F17" s="30">
+      <c r="F17" s="10">
         <v>2484</v>
       </c>
-      <c r="G17" s="30">
+      <c r="G17" s="10">
         <v>1107</v>
       </c>
-      <c r="H17" s="30">
+      <c r="H17" s="10">
         <v>1350</v>
       </c>
-      <c r="I17" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J17" s="31">
+      <c r="I17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="11">
         <v>6</v>
       </c>
-      <c r="K17" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L17" s="30">
+      <c r="K17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="10">
         <v>21</v>
       </c>
-      <c r="M17" s="31">
+      <c r="M17" s="11">
         <v>96</v>
       </c>
-      <c r="N17" s="30">
+      <c r="N17" s="10">
         <v>645</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="13">
         <v>2020</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="14">
         <v>5127</v>
       </c>
-      <c r="F18" s="34">
+      <c r="F18" s="14">
         <v>4095</v>
       </c>
-      <c r="G18" s="34">
+      <c r="G18" s="14">
         <v>1854</v>
       </c>
-      <c r="H18" s="34">
+      <c r="H18" s="14">
         <v>2205</v>
       </c>
-      <c r="I18" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="31">
+      <c r="I18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="11">
         <v>6</v>
       </c>
-      <c r="K18" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L18" s="34">
+      <c r="K18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="14">
         <v>33</v>
       </c>
-      <c r="M18" s="30">
+      <c r="M18" s="10">
         <v>132</v>
       </c>
-      <c r="N18" s="34">
+      <c r="N18" s="14">
         <v>897</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="29">
+      <c r="D19" s="9">
         <v>2019</v>
       </c>
-      <c r="E19" s="30">
+      <c r="E19" s="10">
         <v>2622</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="10">
         <v>2184</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="10">
         <v>1035</v>
       </c>
-      <c r="H19" s="30">
+      <c r="H19" s="10">
         <v>873</v>
       </c>
-      <c r="I19" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="31">
+      <c r="I19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J19" s="11">
         <v>231</v>
       </c>
-      <c r="K19" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L19" s="30">
+      <c r="K19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="10">
         <v>48</v>
       </c>
-      <c r="M19" s="31">
+      <c r="M19" s="11">
         <v>54</v>
       </c>
-      <c r="N19" s="30">
+      <c r="N19" s="10">
         <v>384</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="29">
+      <c r="D20" s="9">
         <v>2019</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="10">
         <v>3597</v>
       </c>
-      <c r="F20" s="30">
+      <c r="F20" s="10">
         <v>2757</v>
       </c>
-      <c r="G20" s="30">
+      <c r="G20" s="10">
         <v>1272</v>
       </c>
-      <c r="H20" s="30">
+      <c r="H20" s="10">
         <v>1242</v>
       </c>
-      <c r="I20" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="31">
+      <c r="I20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="11">
         <v>108</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K20" s="11">
         <v>21</v>
       </c>
-      <c r="L20" s="30">
+      <c r="L20" s="10">
         <v>114</v>
       </c>
-      <c r="M20" s="31">
+      <c r="M20" s="11">
         <v>117</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="10">
         <v>726</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="13">
         <v>2019</v>
       </c>
-      <c r="E21" s="34">
+      <c r="E21" s="14">
         <v>6219</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="14">
         <v>4941</v>
       </c>
-      <c r="G21" s="34">
+      <c r="G21" s="14">
         <v>2307</v>
       </c>
-      <c r="H21" s="34">
+      <c r="H21" s="14">
         <v>2115</v>
       </c>
-      <c r="I21" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21" s="30">
+      <c r="I21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="10">
         <v>336</v>
       </c>
-      <c r="K21" s="30">
+      <c r="K21" s="10">
         <v>21</v>
       </c>
-      <c r="L21" s="34">
+      <c r="L21" s="14">
         <v>159</v>
       </c>
-      <c r="M21" s="30">
+      <c r="M21" s="10">
         <v>168</v>
       </c>
-      <c r="N21" s="34">
+      <c r="N21" s="14">
         <v>1107</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="29">
+      <c r="D22" s="9">
         <v>2019</v>
       </c>
-      <c r="E22" s="30">
+      <c r="E22" s="10">
         <v>1785</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="10">
         <v>1518</v>
       </c>
-      <c r="G22" s="30">
+      <c r="G22" s="10">
         <v>663</v>
       </c>
-      <c r="H22" s="30">
+      <c r="H22" s="10">
         <v>837</v>
       </c>
-      <c r="I22" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L22" s="30">
+      <c r="I22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L22" s="10">
         <v>15</v>
       </c>
-      <c r="M22" s="31">
+      <c r="M22" s="11">
         <v>30</v>
       </c>
-      <c r="N22" s="30">
+      <c r="N22" s="10">
         <v>237</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="9">
         <v>2019</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E23" s="10">
         <v>2712</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="10">
         <v>2100</v>
       </c>
-      <c r="G23" s="30">
+      <c r="G23" s="10">
         <v>987</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="10">
         <v>1083</v>
       </c>
-      <c r="I23" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J23" s="31">
+      <c r="I23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" s="11">
         <v>9</v>
       </c>
-      <c r="K23" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L23" s="30">
+      <c r="K23" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="10">
         <v>18</v>
       </c>
-      <c r="M23" s="31">
+      <c r="M23" s="11">
         <v>87</v>
       </c>
-      <c r="N23" s="30">
+      <c r="N23" s="10">
         <v>525</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="13">
         <v>2019</v>
       </c>
-      <c r="E24" s="34">
+      <c r="E24" s="14">
         <v>4497</v>
       </c>
-      <c r="F24" s="34">
+      <c r="F24" s="14">
         <v>3615</v>
       </c>
-      <c r="G24" s="34">
+      <c r="G24" s="14">
         <v>1650</v>
       </c>
-      <c r="H24" s="34">
+      <c r="H24" s="14">
         <v>1923</v>
       </c>
-      <c r="I24" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J24" s="31">
+      <c r="I24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" s="11">
         <v>9</v>
       </c>
-      <c r="K24" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L24" s="34">
+      <c r="K24" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24" s="14">
         <v>36</v>
       </c>
-      <c r="M24" s="30">
+      <c r="M24" s="10">
         <v>117</v>
       </c>
-      <c r="N24" s="34">
+      <c r="N24" s="14">
         <v>765</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="16">
         <v>2018</v>
       </c>
-      <c r="E25" s="30">
+      <c r="E25" s="10">
         <v>2112</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="10">
         <v>1707</v>
       </c>
-      <c r="G25" s="30">
+      <c r="G25" s="10">
         <v>888</v>
       </c>
-      <c r="H25" s="30">
+      <c r="H25" s="10">
         <v>492</v>
       </c>
-      <c r="I25" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J25" s="31">
+      <c r="I25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" s="11">
         <v>303</v>
       </c>
-      <c r="K25" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L25" s="30">
+      <c r="K25" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="10">
         <v>24</v>
       </c>
-      <c r="M25" s="31">
+      <c r="M25" s="11">
         <v>72</v>
       </c>
-      <c r="N25" s="30">
+      <c r="N25" s="10">
         <v>333</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="36">
+      <c r="D26" s="16">
         <v>2018</v>
       </c>
-      <c r="E26" s="30">
+      <c r="E26" s="10">
         <v>2466</v>
       </c>
-      <c r="F26" s="30">
+      <c r="F26" s="10">
         <v>1845</v>
       </c>
-      <c r="G26" s="30">
+      <c r="G26" s="10">
         <v>975</v>
       </c>
-      <c r="H26" s="30">
+      <c r="H26" s="10">
         <v>645</v>
       </c>
-      <c r="I26" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J26" s="31">
+      <c r="I26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" s="11">
         <v>108</v>
       </c>
-      <c r="K26" s="31">
+      <c r="K26" s="11">
         <v>18</v>
       </c>
-      <c r="L26" s="30">
+      <c r="L26" s="10">
         <v>96</v>
       </c>
-      <c r="M26" s="31">
+      <c r="M26" s="11">
         <v>96</v>
       </c>
-      <c r="N26" s="30">
+      <c r="N26" s="10">
         <v>525</v>
       </c>
     </row>
-    <row r="27" spans="2:14" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="37" t="s">
+    <row r="27" spans="2:14" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="38">
+      <c r="D27" s="18">
         <v>2018</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="14">
         <v>4578</v>
       </c>
-      <c r="F27" s="34">
+      <c r="F27" s="14">
         <v>3552</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="14">
         <v>1863</v>
       </c>
-      <c r="H27" s="34">
+      <c r="H27" s="14">
         <v>1137</v>
       </c>
-      <c r="I27" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J27" s="30">
+      <c r="I27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="10">
         <v>411</v>
       </c>
-      <c r="K27" s="30">
+      <c r="K27" s="10">
         <v>18</v>
       </c>
-      <c r="L27" s="34">
+      <c r="L27" s="14">
         <v>120</v>
       </c>
-      <c r="M27" s="30">
+      <c r="M27" s="10">
         <v>171</v>
       </c>
-      <c r="N27" s="34">
+      <c r="N27" s="14">
         <v>858</v>
       </c>
     </row>
     <row r="28" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="16">
         <v>2018</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="10">
         <v>1179</v>
       </c>
-      <c r="F28" s="30">
+      <c r="F28" s="10">
         <v>951</v>
       </c>
-      <c r="G28" s="30">
+      <c r="G28" s="10">
         <v>480</v>
       </c>
-      <c r="H28" s="30">
+      <c r="H28" s="10">
         <v>462</v>
       </c>
-      <c r="I28" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K28" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L28" s="30">
+      <c r="I28" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" s="10">
         <v>6</v>
       </c>
-      <c r="M28" s="31">
+      <c r="M28" s="11">
         <v>72</v>
       </c>
-      <c r="N28" s="30">
+      <c r="N28" s="10">
         <v>198</v>
       </c>
     </row>
     <row r="29" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="36">
+      <c r="D29" s="16">
         <v>2018</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="10">
         <v>1710</v>
       </c>
-      <c r="F29" s="30">
+      <c r="F29" s="10">
         <v>1293</v>
       </c>
-      <c r="G29" s="30">
+      <c r="G29" s="10">
         <v>750</v>
       </c>
-      <c r="H29" s="30">
+      <c r="H29" s="10">
         <v>528</v>
       </c>
-      <c r="I29" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J29" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L29" s="30">
+      <c r="I29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L29" s="10">
         <v>12</v>
       </c>
-      <c r="M29" s="31">
+      <c r="M29" s="11">
         <v>96</v>
       </c>
-      <c r="N29" s="30">
+      <c r="N29" s="10">
         <v>369</v>
       </c>
     </row>
     <row r="30" spans="2:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D30" s="18">
         <v>2018</v>
       </c>
-      <c r="E30" s="34">
+      <c r="E30" s="14">
         <v>2889</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30" s="14">
         <v>2244</v>
       </c>
-      <c r="G30" s="34">
+      <c r="G30" s="14">
         <v>1230</v>
       </c>
-      <c r="H30" s="34">
+      <c r="H30" s="14">
         <v>990</v>
       </c>
-      <c r="I30" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J30" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K30" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L30" s="34">
+      <c r="I30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L30" s="14">
         <v>18</v>
       </c>
-      <c r="M30" s="30">
+      <c r="M30" s="10">
         <v>171</v>
       </c>
-      <c r="N30" s="34">
+      <c r="N30" s="14">
         <v>567</v>
       </c>
     </row>
     <row r="31" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="36">
+      <c r="D31" s="16">
         <v>2017</v>
       </c>
-      <c r="E31" s="30">
+      <c r="E31" s="10">
         <v>1770</v>
       </c>
-      <c r="F31" s="30">
+      <c r="F31" s="10">
         <v>1443</v>
       </c>
-      <c r="G31" s="30">
+      <c r="G31" s="10">
         <v>852</v>
       </c>
-      <c r="H31" s="30">
+      <c r="H31" s="10">
         <v>309</v>
       </c>
-      <c r="I31" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J31" s="30">
+      <c r="I31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J31" s="10">
         <v>258</v>
       </c>
-      <c r="K31" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L31" s="30">
+      <c r="K31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" s="10">
         <v>24</v>
       </c>
-      <c r="M31" s="30">
+      <c r="M31" s="10">
         <v>51</v>
       </c>
-      <c r="N31" s="30">
+      <c r="N31" s="10">
         <v>279</v>
       </c>
     </row>
     <row r="32" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="36">
+      <c r="D32" s="16">
         <v>2017</v>
       </c>
-      <c r="E32" s="30">
+      <c r="E32" s="10">
         <v>1818</v>
       </c>
-      <c r="F32" s="30">
+      <c r="F32" s="10">
         <v>1404</v>
       </c>
-      <c r="G32" s="30">
+      <c r="G32" s="10">
         <v>855</v>
       </c>
-      <c r="H32" s="30">
+      <c r="H32" s="10">
         <v>381</v>
       </c>
-      <c r="I32" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J32" s="30">
+      <c r="I32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" s="10">
         <v>60</v>
       </c>
-      <c r="K32" s="30">
+      <c r="K32" s="10">
         <v>18</v>
       </c>
-      <c r="L32" s="30">
+      <c r="L32" s="10">
         <v>90</v>
       </c>
-      <c r="M32" s="30">
+      <c r="M32" s="10">
         <v>66</v>
       </c>
-      <c r="N32" s="30">
+      <c r="N32" s="10">
         <v>345</v>
       </c>
     </row>
-    <row r="33" spans="2:23" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="37" t="s">
+    <row r="33" spans="2:23" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="38">
+      <c r="D33" s="18">
         <v>2017</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="14">
         <v>3588</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="14">
         <v>2847</v>
       </c>
-      <c r="G33" s="34">
+      <c r="G33" s="14">
         <v>1707</v>
       </c>
-      <c r="H33" s="34">
+      <c r="H33" s="14">
         <v>687</v>
       </c>
-      <c r="I33" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J33" s="30">
+      <c r="I33" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" s="10">
         <v>318</v>
       </c>
-      <c r="K33" s="30">
+      <c r="K33" s="10">
         <v>18</v>
       </c>
-      <c r="L33" s="34">
+      <c r="L33" s="14">
         <v>117</v>
       </c>
-      <c r="M33" s="30">
+      <c r="M33" s="10">
         <v>117</v>
       </c>
-      <c r="N33" s="34">
+      <c r="N33" s="14">
         <v>624</v>
       </c>
     </row>
     <row r="34" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="36">
+      <c r="D34" s="16">
         <v>2017</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="10">
         <v>843</v>
       </c>
-      <c r="F34" s="30">
+      <c r="F34" s="10">
         <v>711</v>
       </c>
-      <c r="G34" s="30">
+      <c r="G34" s="10">
         <v>417</v>
       </c>
-      <c r="H34" s="30">
+      <c r="H34" s="10">
         <v>285</v>
       </c>
-      <c r="I34" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J34" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K34" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L34" s="30">
+      <c r="I34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L34" s="10">
         <v>9</v>
       </c>
-      <c r="M34" s="30">
+      <c r="M34" s="10">
         <v>27</v>
       </c>
-      <c r="N34" s="30">
+      <c r="N34" s="10">
         <v>102</v>
       </c>
     </row>
     <row r="35" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="36">
+      <c r="D35" s="16">
         <v>2017</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E35" s="10">
         <v>1230</v>
       </c>
-      <c r="F35" s="30">
+      <c r="F35" s="10">
         <v>948</v>
       </c>
-      <c r="G35" s="30">
+      <c r="G35" s="10">
         <v>642</v>
       </c>
-      <c r="H35" s="30">
+      <c r="H35" s="10">
         <v>297</v>
       </c>
-      <c r="I35" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J35" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K35" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L35" s="30">
+      <c r="I35" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L35" s="10">
         <v>9</v>
       </c>
-      <c r="M35" s="30">
+      <c r="M35" s="10">
         <v>36</v>
       </c>
-      <c r="N35" s="30">
+      <c r="N35" s="10">
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="2:23" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="37" t="s">
+    <row r="36" spans="2:23" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="38">
+      <c r="D36" s="18">
         <v>2017</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="14">
         <v>2070</v>
       </c>
-      <c r="F36" s="34">
+      <c r="F36" s="14">
         <v>1659</v>
       </c>
-      <c r="G36" s="34">
+      <c r="G36" s="14">
         <v>1059</v>
       </c>
-      <c r="H36" s="34">
+      <c r="H36" s="14">
         <v>582</v>
       </c>
-      <c r="I36" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J36" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="K36" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L36" s="34">
+      <c r="I36" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L36" s="14">
         <v>18</v>
       </c>
-      <c r="M36" s="30">
+      <c r="M36" s="10">
         <v>63</v>
       </c>
-      <c r="N36" s="34">
+      <c r="N36" s="14">
         <v>348</v>
       </c>
     </row>
     <row r="37" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="36">
+      <c r="D37" s="16">
         <v>2016</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="10">
         <v>1620</v>
       </c>
-      <c r="F37" s="30">
+      <c r="F37" s="10">
         <v>1320</v>
       </c>
-      <c r="G37" s="30">
+      <c r="G37" s="10">
         <v>891</v>
       </c>
-      <c r="H37" s="30">
+      <c r="H37" s="10">
         <v>243</v>
       </c>
-      <c r="I37" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J37" s="30">
+      <c r="I37" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J37" s="10">
         <v>159</v>
       </c>
-      <c r="K37" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L37" s="30">
+      <c r="K37" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L37" s="10">
         <v>27</v>
       </c>
-      <c r="M37" s="30">
+      <c r="M37" s="10">
         <v>51</v>
       </c>
-      <c r="N37" s="30">
+      <c r="N37" s="10">
         <v>252</v>
       </c>
-      <c r="O37" s="30"/>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30"/>
-      <c r="R37" s="30"/>
-      <c r="S37" s="30"/>
-      <c r="T37" s="30"/>
-      <c r="U37" s="30"/>
-      <c r="V37" s="30"/>
-      <c r="W37" s="30"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
     </row>
     <row r="38" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D38" s="36">
+      <c r="D38" s="16">
         <v>2016</v>
       </c>
-      <c r="E38" s="30">
+      <c r="E38" s="10">
         <v>1737</v>
       </c>
-      <c r="F38" s="30">
+      <c r="F38" s="10">
         <v>1362</v>
       </c>
-      <c r="G38" s="30">
+      <c r="G38" s="10">
         <v>831</v>
       </c>
-      <c r="H38" s="30">
+      <c r="H38" s="10">
         <v>372</v>
       </c>
-      <c r="I38" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J38" s="30">
+      <c r="I38" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J38" s="10">
         <v>75</v>
       </c>
-      <c r="K38" s="30">
+      <c r="K38" s="10">
         <v>3</v>
       </c>
-      <c r="L38" s="30">
+      <c r="L38" s="10">
         <v>78</v>
       </c>
-      <c r="M38" s="30">
+      <c r="M38" s="10">
         <v>66</v>
       </c>
-      <c r="N38" s="30">
+      <c r="N38" s="10">
         <v>309</v>
       </c>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="30"/>
-      <c r="S38" s="30"/>
-      <c r="T38" s="30"/>
-      <c r="U38" s="30"/>
-      <c r="V38" s="30"/>
-      <c r="W38" s="30"/>
-    </row>
-    <row r="39" spans="2:23" s="40" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="37" t="s">
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+    </row>
+    <row r="39" spans="2:23" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="38">
+      <c r="D39" s="18">
         <v>2016</v>
       </c>
-      <c r="E39" s="34">
+      <c r="E39" s="14">
         <v>3360</v>
       </c>
-      <c r="F39" s="34">
+      <c r="F39" s="14">
         <v>2682</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G39" s="14">
         <v>1722</v>
       </c>
-      <c r="H39" s="34">
+      <c r="H39" s="14">
         <v>615</v>
       </c>
-      <c r="I39" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J39" s="30">
+      <c r="I39" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J39" s="10">
         <v>234</v>
       </c>
-      <c r="K39" s="30">
+      <c r="K39" s="10">
         <v>6</v>
       </c>
-      <c r="L39" s="34">
+      <c r="L39" s="14">
         <v>105</v>
       </c>
-      <c r="M39" s="30">
+      <c r="M39" s="10">
         <v>117</v>
       </c>
-      <c r="N39" s="34">
+      <c r="N39" s="14">
         <v>561</v>
       </c>
-      <c r="O39" s="34"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="34"/>
-      <c r="U39" s="34"/>
-      <c r="V39" s="34"/>
-      <c r="W39" s="34"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="14"/>
+      <c r="R39" s="14"/>
+      <c r="S39" s="14"/>
+      <c r="T39" s="14"/>
+      <c r="U39" s="14"/>
+      <c r="V39" s="14"/>
+      <c r="W39" s="14"/>
     </row>
     <row r="40" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="36">
+      <c r="D40" s="16">
         <v>2016</v>
       </c>
-      <c r="E40" s="30">
+      <c r="E40" s="10">
         <v>798</v>
       </c>
-      <c r="F40" s="30">
+      <c r="F40" s="10">
         <v>711</v>
       </c>
-      <c r="G40" s="30">
+      <c r="G40" s="10">
         <v>486</v>
       </c>
-      <c r="H40" s="30">
+      <c r="H40" s="10">
         <v>222</v>
       </c>
-      <c r="I40" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J40" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="K40" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L40" s="30">
+      <c r="I40" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L40" s="10">
         <v>3</v>
       </c>
-      <c r="M40" s="30">
+      <c r="M40" s="10">
         <v>12</v>
       </c>
-      <c r="N40" s="30">
+      <c r="N40" s="10">
         <v>72</v>
       </c>
-      <c r="O40" s="30"/>
-      <c r="P40" s="30"/>
-      <c r="Q40" s="30"/>
-      <c r="R40" s="30"/>
-      <c r="S40" s="30"/>
-      <c r="T40" s="30"/>
-      <c r="U40" s="30"/>
-      <c r="V40" s="30"/>
-      <c r="W40" s="30"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
     </row>
     <row r="41" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D41" s="36">
+      <c r="D41" s="16">
         <v>2016</v>
       </c>
-      <c r="E41" s="30">
+      <c r="E41" s="10">
         <v>1071</v>
       </c>
-      <c r="F41" s="30">
+      <c r="F41" s="10">
         <v>903</v>
       </c>
-      <c r="G41" s="30">
+      <c r="G41" s="10">
         <v>612</v>
       </c>
-      <c r="H41" s="30">
+      <c r="H41" s="10">
         <v>282</v>
       </c>
-      <c r="I41" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J41" s="30">
+      <c r="I41" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J41" s="10">
         <v>3</v>
       </c>
-      <c r="K41" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L41" s="30">
+      <c r="K41" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L41" s="10">
         <v>6</v>
       </c>
-      <c r="M41" s="30">
+      <c r="M41" s="10">
         <v>21</v>
       </c>
-      <c r="N41" s="30">
+      <c r="N41" s="10">
         <v>144</v>
       </c>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="S41" s="30"/>
-      <c r="T41" s="30"/>
-      <c r="U41" s="30"/>
-      <c r="V41" s="30"/>
-      <c r="W41" s="30"/>
-    </row>
-    <row r="42" spans="2:23" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="37" t="s">
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10"/>
+      <c r="W41" s="10"/>
+    </row>
+    <row r="42" spans="2:23" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="41">
+      <c r="D42" s="21">
         <v>2016</v>
       </c>
-      <c r="E42" s="42">
+      <c r="E42" s="22">
         <v>1869</v>
       </c>
-      <c r="F42" s="42">
+      <c r="F42" s="22">
         <v>1614</v>
       </c>
-      <c r="G42" s="42">
+      <c r="G42" s="22">
         <v>1098</v>
       </c>
-      <c r="H42" s="42">
+      <c r="H42" s="22">
         <v>504</v>
       </c>
-      <c r="I42" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="J42" s="30">
+      <c r="I42" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J42" s="10">
         <v>3</v>
       </c>
-      <c r="K42" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="L42" s="42">
+      <c r="K42" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L42" s="22">
         <v>9</v>
       </c>
-      <c r="M42" s="30">
+      <c r="M42" s="10">
         <v>36</v>
       </c>
-      <c r="N42" s="42">
+      <c r="N42" s="22">
         <v>219</v>
       </c>
-      <c r="O42" s="42"/>
-      <c r="P42" s="42"/>
-      <c r="Q42" s="42"/>
-      <c r="R42" s="42"/>
-      <c r="S42" s="42"/>
-      <c r="T42" s="42"/>
-      <c r="U42" s="42"/>
-      <c r="V42" s="42"/>
-      <c r="W42" s="42"/>
+      <c r="O42" s="22"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22"/>
+      <c r="T42" s="22"/>
+      <c r="U42" s="22"/>
+      <c r="V42" s="22"/>
+      <c r="W42" s="22"/>
     </row>
     <row r="43" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="43">
+      <c r="D43" s="23">
         <v>2015</v>
       </c>
-      <c r="E43" s="44">
+      <c r="E43" s="24">
         <v>1098</v>
       </c>
-      <c r="F43" s="44">
+      <c r="F43" s="24">
         <v>957</v>
       </c>
-      <c r="G43" s="44">
+      <c r="G43" s="24">
         <v>660</v>
       </c>
-      <c r="H43" s="44">
+      <c r="H43" s="24">
         <v>198</v>
       </c>
-      <c r="I43" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L43" s="44">
+      <c r="I43" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" s="24">
         <v>105</v>
       </c>
-      <c r="N43" s="44">
+      <c r="N43" s="24">
         <v>135</v>
       </c>
     </row>
     <row r="44" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D44" s="43">
+      <c r="D44" s="23">
         <v>2015</v>
       </c>
-      <c r="E44" s="44">
+      <c r="E44" s="24">
         <v>1506</v>
       </c>
-      <c r="F44" s="44">
+      <c r="F44" s="24">
         <v>1227</v>
       </c>
-      <c r="G44" s="44">
+      <c r="G44" s="24">
         <v>669</v>
       </c>
-      <c r="H44" s="44">
+      <c r="H44" s="24">
         <v>372</v>
       </c>
-      <c r="I44" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L44" s="44">
+      <c r="I44" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" s="24">
         <v>180</v>
       </c>
-      <c r="N44" s="44">
+      <c r="N44" s="24">
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="2:23" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="37" t="s">
+    <row r="45" spans="2:23" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C45" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D45" s="37">
+      <c r="D45" s="17">
         <v>2015</v>
       </c>
-      <c r="E45" s="45">
+      <c r="E45" s="25">
         <v>2616</v>
       </c>
-      <c r="F45" s="45">
+      <c r="F45" s="25">
         <v>2199</v>
       </c>
-      <c r="G45" s="45">
+      <c r="G45" s="25">
         <v>1335</v>
       </c>
-      <c r="H45" s="45">
+      <c r="H45" s="25">
         <v>573</v>
       </c>
-      <c r="I45" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="L45" s="45">
+      <c r="I45" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L45" s="25">
         <v>291</v>
       </c>
-      <c r="N45" s="45">
+      <c r="N45" s="25">
         <v>414</v>
       </c>
     </row>
     <row r="46" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C46" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="43">
+      <c r="D46" s="23">
         <v>2015</v>
       </c>
-      <c r="E46" s="44">
+      <c r="E46" s="24">
         <v>648</v>
       </c>
-      <c r="F46" s="44">
+      <c r="F46" s="24">
         <v>591</v>
       </c>
-      <c r="G46" s="44">
+      <c r="G46" s="24">
         <v>396</v>
       </c>
-      <c r="I46" s="44">
+      <c r="I46" s="24">
         <v>183</v>
       </c>
-      <c r="L46" s="44">
+      <c r="L46" s="24">
         <v>12</v>
       </c>
-      <c r="N46" s="44">
+      <c r="N46" s="24">
         <v>57</v>
       </c>
     </row>
     <row r="47" spans="2:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="43">
+      <c r="D47" s="23">
         <v>2015</v>
       </c>
-      <c r="E47" s="44">
+      <c r="E47" s="24">
         <v>885</v>
       </c>
-      <c r="F47" s="44">
+      <c r="F47" s="24">
         <v>702</v>
       </c>
-      <c r="G47" s="44">
+      <c r="G47" s="24">
         <v>441</v>
       </c>
-      <c r="I47" s="44">
+      <c r="I47" s="24">
         <v>225</v>
       </c>
-      <c r="L47" s="44">
+      <c r="L47" s="24">
         <v>36</v>
       </c>
-      <c r="N47" s="44">
+      <c r="N47" s="24">
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="2:23" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="37" t="s">
+    <row r="48" spans="2:23" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="37" t="s">
+      <c r="C48" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="37">
+      <c r="D48" s="17">
         <v>2015</v>
       </c>
-      <c r="E48" s="45">
+      <c r="E48" s="25">
         <v>1530</v>
       </c>
-      <c r="F48" s="45">
+      <c r="F48" s="25">
         <v>1293</v>
       </c>
-      <c r="G48" s="45">
+      <c r="G48" s="25">
         <v>837</v>
       </c>
-      <c r="I48" s="45">
+      <c r="I48" s="25">
         <v>408</v>
       </c>
-      <c r="L48" s="45">
+      <c r="L48" s="25">
         <v>48</v>
       </c>
-      <c r="N48" s="45">
+      <c r="N48" s="25">
         <v>237</v>
       </c>
     </row>
     <row r="49" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C49" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="43">
+      <c r="D49" s="23">
         <v>2014</v>
       </c>
-      <c r="E49" s="46">
+      <c r="E49" s="26">
         <v>1005</v>
       </c>
-      <c r="F49" s="46">
+      <c r="F49" s="26">
         <v>916</v>
       </c>
-      <c r="G49" s="46">
+      <c r="G49" s="26">
         <v>600</v>
       </c>
-      <c r="I49" s="46">
+      <c r="I49" s="26">
         <v>221</v>
       </c>
-      <c r="L49" s="46">
+      <c r="L49" s="26">
         <v>95</v>
       </c>
-      <c r="N49" s="46">
+      <c r="N49" s="26">
         <v>89</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C50" s="35" t="s">
+      <c r="C50" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D50" s="43">
+      <c r="D50" s="23">
         <v>2014</v>
       </c>
-      <c r="E50" s="46">
+      <c r="E50" s="26">
         <v>1665</v>
       </c>
-      <c r="F50" s="46">
+      <c r="F50" s="26">
         <v>1248</v>
       </c>
-      <c r="G50" s="46">
+      <c r="G50" s="26">
         <v>851</v>
       </c>
-      <c r="I50" s="46">
+      <c r="I50" s="26">
         <v>279</v>
       </c>
-      <c r="L50" s="46">
+      <c r="L50" s="26">
         <v>118</v>
       </c>
-      <c r="N50" s="46">
+      <c r="N50" s="26">
         <v>417</v>
       </c>
     </row>
-    <row r="51" spans="2:14" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="37" t="s">
+    <row r="51" spans="2:14" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="37" t="s">
+      <c r="C51" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D51" s="37">
+      <c r="D51" s="17">
         <v>2014</v>
       </c>
-      <c r="E51" s="47">
+      <c r="E51" s="27">
         <v>2670</v>
       </c>
-      <c r="F51" s="47">
+      <c r="F51" s="27">
         <v>2164</v>
       </c>
-      <c r="G51" s="47">
+      <c r="G51" s="27">
         <v>1451</v>
       </c>
-      <c r="I51" s="47">
+      <c r="I51" s="27">
         <v>500</v>
       </c>
-      <c r="L51" s="47">
+      <c r="L51" s="27">
         <v>213</v>
       </c>
-      <c r="N51" s="47">
+      <c r="N51" s="27">
         <v>506</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="43">
+      <c r="D52" s="23">
         <v>2014</v>
       </c>
-      <c r="E52" s="46">
+      <c r="E52" s="26">
         <v>635</v>
       </c>
-      <c r="F52" s="46">
+      <c r="F52" s="26">
         <v>597</v>
       </c>
-      <c r="G52" s="46">
+      <c r="G52" s="26">
         <v>392</v>
       </c>
-      <c r="I52" s="46">
+      <c r="I52" s="26">
         <v>199</v>
       </c>
-      <c r="L52" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="N52" s="48" t="s">
+      <c r="L52" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="N52" s="28" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="53" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="43">
+      <c r="D53" s="23">
         <v>2014</v>
       </c>
-      <c r="E53" s="46">
+      <c r="E53" s="26">
         <v>730</v>
       </c>
-      <c r="F53" s="46">
+      <c r="F53" s="26">
         <v>544</v>
       </c>
-      <c r="G53" s="46">
+      <c r="G53" s="26">
         <v>369</v>
       </c>
-      <c r="I53" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="L53" s="46">
-        <v>37</v>
-      </c>
-      <c r="N53" s="46">
+      <c r="I53" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="L53" s="26">
+        <v>37</v>
+      </c>
+      <c r="N53" s="26">
         <v>186</v>
       </c>
     </row>
-    <row r="54" spans="2:14" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="37" t="s">
+    <row r="54" spans="2:14" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="37" t="s">
+      <c r="C54" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="37">
+      <c r="D54" s="17">
         <v>2014</v>
       </c>
-      <c r="E54" s="47">
+      <c r="E54" s="27">
         <v>1365</v>
       </c>
-      <c r="F54" s="47">
+      <c r="F54" s="27">
         <v>1141</v>
       </c>
-      <c r="G54" s="47">
+      <c r="G54" s="27">
         <v>761</v>
       </c>
-      <c r="I54" s="47">
+      <c r="I54" s="27">
         <v>199</v>
       </c>
-      <c r="L54" s="47">
-        <v>37</v>
-      </c>
-      <c r="N54" s="47">
+      <c r="L54" s="27">
+        <v>37</v>
+      </c>
+      <c r="N54" s="27">
         <v>186</v>
       </c>
     </row>
     <row r="55" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D55" s="43">
+      <c r="D55" s="23">
+        <v>2013</v>
+      </c>
+      <c r="E55" s="29">
+        <v>261</v>
+      </c>
+      <c r="F55" s="23">
+        <v>222</v>
+      </c>
+      <c r="G55" s="29">
+        <v>12</v>
+      </c>
+      <c r="I55" s="29">
+        <v>6</v>
+      </c>
+      <c r="L55" s="29">
+        <v>204</v>
+      </c>
+      <c r="N55" s="29">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="23">
+        <v>2013</v>
+      </c>
+      <c r="E56" s="29">
+        <v>402</v>
+      </c>
+      <c r="F56" s="23">
+        <v>339</v>
+      </c>
+      <c r="G56" s="29">
+        <v>30</v>
+      </c>
+      <c r="I56" s="29">
+        <v>57</v>
+      </c>
+      <c r="L56" s="29">
+        <v>252</v>
+      </c>
+      <c r="N56" s="29">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D57" s="17">
+        <v>2013</v>
+      </c>
+      <c r="E57" s="30">
+        <v>663</v>
+      </c>
+      <c r="F57" s="17">
+        <v>561</v>
+      </c>
+      <c r="G57" s="30">
+        <v>42</v>
+      </c>
+      <c r="I57" s="30">
+        <v>63</v>
+      </c>
+      <c r="L57" s="30">
+        <v>456</v>
+      </c>
+      <c r="N57" s="30">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="23">
         <v>2012</v>
       </c>
-      <c r="E55" s="49">
-        <v>261</v>
-      </c>
-      <c r="F55" s="43">
-        <v>222</v>
-      </c>
-      <c r="G55" s="49">
+      <c r="E58" s="29">
+        <v>189</v>
+      </c>
+      <c r="F58" s="23">
+        <v>180</v>
+      </c>
+      <c r="G58" s="29">
+        <v>3</v>
+      </c>
+      <c r="I58" s="29">
+        <v>6</v>
+      </c>
+      <c r="L58" s="29">
+        <v>171</v>
+      </c>
+      <c r="N58" s="29">
         <v>12</v>
       </c>
-      <c r="I55" s="49">
-        <v>6</v>
-      </c>
-      <c r="L55" s="49">
-        <v>204</v>
-      </c>
-      <c r="N55" s="49">
+    </row>
+    <row r="59" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="23">
+        <v>2012</v>
+      </c>
+      <c r="E59" s="29">
+        <v>327</v>
+      </c>
+      <c r="F59" s="23">
+        <v>291</v>
+      </c>
+      <c r="G59" s="29">
+        <v>18</v>
+      </c>
+      <c r="I59" s="29">
+        <v>57</v>
+      </c>
+      <c r="L59" s="29">
+        <v>219</v>
+      </c>
+      <c r="N59" s="29">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" s="17">
+        <v>2012</v>
+      </c>
+      <c r="E60" s="30">
+        <v>519</v>
+      </c>
+      <c r="F60" s="17">
+        <v>471</v>
+      </c>
+      <c r="G60" s="30">
+        <v>18</v>
+      </c>
+      <c r="I60" s="30">
+        <v>63</v>
+      </c>
+      <c r="L60" s="30">
+        <v>390</v>
+      </c>
+      <c r="N60" s="30">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="31"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+    </row>
+    <row r="62" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="34" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="56" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="C56" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D56" s="43">
-        <v>2012</v>
-      </c>
-      <c r="E56" s="49">
-        <v>402</v>
-      </c>
-      <c r="F56" s="43">
-        <v>339</v>
-      </c>
-      <c r="G56" s="49">
-        <v>30</v>
-      </c>
-      <c r="I56" s="49">
-        <v>57</v>
-      </c>
-      <c r="L56" s="49">
-        <v>252</v>
-      </c>
-      <c r="N56" s="49">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" s="37">
-        <v>2012</v>
-      </c>
-      <c r="E57" s="50">
-        <v>663</v>
-      </c>
-      <c r="F57" s="37">
-        <v>561</v>
-      </c>
-      <c r="G57" s="50">
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="33"/>
+    </row>
+    <row r="63" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="36"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="33"/>
+    </row>
+    <row r="64" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C64" s="36"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="36"/>
+      <c r="G64" s="36"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="36"/>
+      <c r="J64" s="36"/>
+      <c r="K64" s="36"/>
+      <c r="L64" s="36"/>
+      <c r="M64" s="36"/>
+    </row>
+    <row r="65" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I57" s="50">
-        <v>63</v>
-      </c>
-      <c r="L57" s="50">
-        <v>456</v>
-      </c>
-      <c r="N57" s="50">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="C58" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="43">
-        <v>2012</v>
-      </c>
-      <c r="E58" s="49">
-        <v>189</v>
-      </c>
-      <c r="F58" s="43">
-        <v>180</v>
-      </c>
-      <c r="G58" s="49">
-        <v>3</v>
-      </c>
-      <c r="I58" s="49">
-        <v>6</v>
-      </c>
-      <c r="L58" s="49">
-        <v>171</v>
-      </c>
-      <c r="N58" s="49">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D59" s="43">
-        <v>2012</v>
-      </c>
-      <c r="E59" s="49">
-        <v>327</v>
-      </c>
-      <c r="F59" s="43">
-        <v>291</v>
-      </c>
-      <c r="G59" s="49">
-        <v>18</v>
-      </c>
-      <c r="I59" s="49">
-        <v>57</v>
-      </c>
-      <c r="L59" s="49">
-        <v>219</v>
-      </c>
-      <c r="N59" s="49">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D60" s="37">
-        <v>2012</v>
-      </c>
-      <c r="E60" s="50">
-        <v>519</v>
-      </c>
-      <c r="F60" s="37">
-        <v>471</v>
-      </c>
-      <c r="G60" s="50">
-        <v>18</v>
-      </c>
-      <c r="I60" s="50">
-        <v>63</v>
-      </c>
-      <c r="L60" s="50">
-        <v>390</v>
-      </c>
-      <c r="N60" s="50">
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="33"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="33"/>
+    </row>
+    <row r="66" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33"/>
+    </row>
+    <row r="67" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="36"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="33"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33"/>
+    </row>
+    <row r="68" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="33"/>
+    </row>
+    <row r="69" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="36"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="36"/>
+      <c r="I69" s="33"/>
+      <c r="J69" s="33"/>
+    </row>
+    <row r="70" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="36"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="36"/>
+      <c r="I70" s="33"/>
+      <c r="J70" s="33"/>
+    </row>
+    <row r="71" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="36"/>
+      <c r="D71" s="36"/>
+      <c r="E71" s="36"/>
+      <c r="F71" s="36"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="36"/>
+      <c r="I71" s="33"/>
+      <c r="J71" s="33"/>
+    </row>
+    <row r="72" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="36"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="33"/>
+    </row>
+    <row r="73" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="36"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+    </row>
+    <row r="74" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="37" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="61" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="51"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="53"/>
-      <c r="H61" s="53"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="53"/>
-    </row>
-    <row r="62" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="54" t="s">
-        <v>39</v>
-      </c>
-      <c r="C62" s="55"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="55"/>
-      <c r="H62" s="55"/>
-      <c r="I62" s="53"/>
-      <c r="J62" s="53"/>
-    </row>
-    <row r="63" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="56" t="s">
-        <v>40</v>
-      </c>
-      <c r="C63" s="56"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="56"/>
-      <c r="I63" s="53"/>
-      <c r="J63" s="53"/>
-    </row>
-    <row r="64" spans="2:14" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="C64" s="56"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="56"/>
-      <c r="I64" s="56"/>
-      <c r="J64" s="56"/>
-      <c r="K64" s="56"/>
-      <c r="L64" s="56"/>
-      <c r="M64" s="56"/>
-    </row>
-    <row r="65" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="C65" s="52"/>
-      <c r="D65" s="52"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="52"/>
-      <c r="G65" s="53"/>
-      <c r="H65" s="53"/>
-      <c r="I65" s="53"/>
-      <c r="J65" s="53"/>
-    </row>
-    <row r="66" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="C66" s="52"/>
-      <c r="D66" s="52"/>
-      <c r="E66" s="53"/>
-      <c r="F66" s="52"/>
-      <c r="G66" s="53"/>
-      <c r="H66" s="53"/>
-      <c r="I66" s="53"/>
-      <c r="J66" s="53"/>
-    </row>
-    <row r="67" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="56"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="52"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="52"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="53"/>
-      <c r="I67" s="53"/>
-      <c r="J67" s="53"/>
-    </row>
-    <row r="68" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C68" s="52"/>
-      <c r="D68" s="52"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="52"/>
-      <c r="G68" s="53"/>
-      <c r="H68" s="53"/>
-      <c r="I68" s="53"/>
-      <c r="J68" s="53"/>
-    </row>
-    <row r="69" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="56"/>
-      <c r="C69" s="56"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
-      <c r="H69" s="56"/>
-      <c r="I69" s="53"/>
-      <c r="J69" s="53"/>
-    </row>
-    <row r="70" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="56"/>
-      <c r="C70" s="56"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="56"/>
-      <c r="I70" s="53"/>
-      <c r="J70" s="53"/>
-    </row>
-    <row r="71" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="56" t="s">
-        <v>45</v>
-      </c>
-      <c r="C71" s="56"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="56"/>
-      <c r="I71" s="53"/>
-      <c r="J71" s="53"/>
-    </row>
-    <row r="72" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="C72" s="56"/>
-      <c r="D72" s="56"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56"/>
-      <c r="G72" s="56"/>
-      <c r="H72" s="56"/>
-      <c r="I72" s="53"/>
-      <c r="J72" s="53"/>
-    </row>
-    <row r="73" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="C73" s="56"/>
-      <c r="D73" s="56"/>
-      <c r="E73" s="56"/>
-      <c r="F73" s="56"/>
-      <c r="G73" s="56"/>
-      <c r="H73" s="56"/>
-      <c r="I73" s="53"/>
-      <c r="J73" s="53"/>
-    </row>
-    <row r="74" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="C74" s="56"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56"/>
-      <c r="G74" s="56"/>
-      <c r="H74" s="56"/>
-      <c r="I74" s="53"/>
-      <c r="J74" s="53"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="36"/>
+      <c r="G74" s="36"/>
+      <c r="H74" s="36"/>
+      <c r="I74" s="33"/>
+      <c r="J74" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C10:N10"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B6:N6"/>
     <mergeCell ref="B7:B10"/>
@@ -3188,6 +3181,13 @@
     <mergeCell ref="M7:M9"/>
     <mergeCell ref="N7:N9"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="C10:N10"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B74" r:id="rId1" xr:uid="{3ADF4A85-3A7E-422B-BEA1-45B48965058B}"/>

</xml_diff>